<commit_message>
removed randbytes import from speakqlpredictorcaller
</commit_message>
<xml_diff>
--- a/generated_query_pairs.xlsx
+++ b/generated_query_pairs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>SQL</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -459,6 +464,11 @@
           <t xml:space="preserve">SELECT CITY.COUNTRYCODE, CITY.ID, COUNTRY.REGION, CY.CONTINENT FROM CITY NATURAL JOIN COUNTRY AS CY WHERE(CY.COUNTRY_ID &lt; &gt; 'REPOSITORY' AND CY.CAPITAL &gt; 2058) ORDER BY CONTINENT DESC LIMIT 31 </t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -474,6 +484,11 @@
           <t xml:space="preserve">IN FROM TABLE COURSE WHERE CODE = 'SWORE' RETRIEVE THE COUNT UNITS AND UNITS AND COUNT UNITS GROUP AUTOMATIC HAVING MIN UNITS &lt; &gt; 157 AS TERM WHERE ENDDATE = '1965-5-15' OR ID = 'SINFUL' DISPLAY SUM YEAR AND TERM.STARTDATE LIMIT 12 GROUP BY AUTOMATIC HAVING MIN STARTDATE &gt; 131 </t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PARTIAL ERROR</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -489,6 +504,11 @@
           <t xml:space="preserve">SELECT CITY, CITY.LAST_UPDATE FROM CITY AS CY WHERE CITY &lt; &gt; 'ASPLENIUM' OR COUNTRY_ID = 'SPILL' HAVING MAX(CITY) &lt; &gt; 66 LIMIT 11 </t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -504,6 +524,11 @@
           <t xml:space="preserve">SELECT CITY.CITY_ID, COUNTRY_ID FROM CITY AS CY WHERE CITY = 'COLOSSI' AND CITY IN(SELECT ID FROM CITY) LIMIT 34 </t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -519,6 +544,11 @@
           <t xml:space="preserve">SELECT COUNT(COUNTRY_ID), CITY.DISTRICT FROM CITY WHERE COUNTRY_ID = 'PENUMBRA' OR COUNTRY_ID = 'ANAGLYPH' GROUP BY CITY.DISTRICT HAVING SUM(DISTRICT) &lt; &gt; 145 LIMIT 49 </t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -534,6 +564,11 @@
           <t xml:space="preserve">SELECT CAPACITY, COURSEOFFERING.COURSEID, COURSEOFFERING.FACULTYNAME FROM COURSEOFFERING AS CG HAVING SUM(CAPACITY) &lt; &gt; 2 </t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -549,6 +584,11 @@
           <t xml:space="preserve">SELECT PT.STAFF_ID, COUNT(DISTINCT PT.CUSTOMER_ID), COUNT(DISTINCT RL.LAST_UPDATE), RENTAL.RETURN_DATE, RENTAL.INVENTORY_ID, INVENTORY.LAST_UPDATE, INVENTORY.STORE_ID, INVENTORY.FILM_ID, INVENTORY.INVENTORY_ID, _TN_._TNCN_, INVENTORY._CN_, STORE.MANAGER_STAFF_ID, SE.ADDRESS_ID, STORE.STORE_ID, SE.LAST_UPDATE FROM PAYMENT AS PT NATURAL JOIN RENTAL AS RL NATURAL JOIN INVENTORY NATURAL JOIN STORE AS SE WHERE(PT.PAYMENT_ID = 'PERMISSION' OR PT.CUSTOMER_ID &lt; &gt; 'EXOTICA') AND(SE.STORE_ID &lt; &gt; 'GRIDDLE' AND SE.MANAGER_STAFF_ID = 'RUANDA') GROUP BY PT.STAFF_ID, RENTAL.RETURN_DATE, RENTAL.INVENTORY_ID, INVENTORY.LAST_UPDATE, INVENTORY.STORE_ID, INVENTORY.FILM_ID, INVENTORY.INVENTORY_ID, _TN_._TNCN_, INVENTORY._CN_, STORE.MANAGER_STAFF_ID, SE.ADDRESS_ID, STORE.STORE_ID, SE.LAST_UPDATE HAVING AVG(ADDRESS_ID) &gt; 185 </t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -564,6 +604,11 @@
           <t xml:space="preserve">SELECT STAFF.LAST_UPDATE, COUNT(SF.FIRST_NAME), COUNT(SF.FIRST_NAME), CITY.DISTRICT, CITY.ID, COUNT(LANGUAGE.LANGUAGE_ID), LANGUAGE.NAME FROM STAFF AS SF NATURAL JOIN ADDRESS NATURAL JOIN CITY NATURAL JOIN(SELECT COUNT(PAYMENT_DATE), PAYMENT.STAFF_ID FROM PAYMENT AS PT GROUP BY PAYMENT.STAFF_ID) AS LANGUAGE WHERE(CITY.NAME = 'INSURRECT' OR CITY.COUNTRY_ID IN(SELECT CITY_ID FROM LANGUAGE)) GROUP BY STAFF.LAST_UPDATE, CITY.DISTRICT, CITY.ID, LANGUAGE.NAME </t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -579,6 +624,11 @@
           <t xml:space="preserve">SELECT MANAGER_STAFF_ID, LAST_UPDATE FROM STORE HAVING AVG(MANAGER_STAFF_ID) &lt; 127 ORDER BY MANAGER_STAFF_ID </t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -594,6 +644,11 @@
           <t xml:space="preserve">SELECT EMPLOYEENUMBER, COUNT(TITLE), TITLES.TODATE FROM TITLES GROUP BY EMPLOYEENUMBER, TITLES.TODATE </t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -609,6 +664,11 @@
           <t xml:space="preserve">JOIN ROOM WITH BUILDING ON ROOM.BUILDINGID EQUALS BUILDING.ID GROUP BY COURSEOFFERING.FACULTYNAME, BUILDING.BUILDINGNAME, BUILDING.ID HAVING AVG(ID) &lt; 185 </t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PARTIAL ERROR</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -624,6 +684,11 @@
           <t xml:space="preserve">SELECT COUNT(ID), CITY.COUNTRY_ID, CITY.CITY_ID FROM CITY WHERE COUNTRY_ID IN(SELECT DISTRICT FROM CITY) OR NAME = 'TRIPE' GROUP BY CITY.COUNTRY_ID, CITY.CITY_ID </t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -639,6 +704,11 @@
           <t xml:space="preserve">SELECT INVENTORY.LAST_UPDATE, INVENTORY.STORE_ID, INVENTORY.FILM_ID, STORE.ADDRESS_ID, COUNT(STORE.MANAGER_STAFF_ID), SF.STORE_ID, SF.LAST_UPDATE FROM(SELECT LAST_UPDATE, COUNT(POPULATION), CITY.CITY_ID FROM CITY WHERE CITY_ID &lt; &gt; 'LOTTERY' OR POPULATION &lt; &gt; 1489 HAVING COUNT(CITY_ID) &lt; 6 GROUP BY LAST_UPDATE, CITY.CITY_ID) AS INVENTORY NATURAL JOIN STORE JOIN STAFF AS SF ON STORE.MANAGER_STAFF_ID WHERE(STORE.MANAGER_STAFF_ID = 'DANGEROUS') AND(SF.FIRST_NAME IN(SELECT LAST_NAME FROM INVENTORY) OR SF.STORE_ID &lt; &gt; 'CHART') </t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -646,12 +716,13 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FIND store . address_id , manager_staff_id where manager_staff_id = 'Eugene' FROM the store table LIMIT 28 HAVING COUNT ( address_id ) &lt; 95</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SELECT STORE.ADDRESS_ID, MANAGER_STAFF_ID FROM STORE WHERE MANAGER_STAFF_ID = 'EUGENE' HAVING COUNT(ADDRESS_ID) &lt; 95 LIMIT 28 </t>
+          <t>natural join address with city AND THEN WHAT IS address . address_id , address . address where district IN ( FIND address IN TABLE address ) FROM table address as as AND THEN IN the city table SELECT city . last_update , avg ( Population ) , max ( Population ) where country_id = 'blemish' AND THEN GROUP AUTOMATICALLY HAVING COUNT ( last_update ) &lt;&gt; 145</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TOTAL ERROR</t>
         </is>
       </c>
     </row>
@@ -661,12 +732,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WHAT ARE THE last_update and city . Population where CountryCode IN ( SELECT District FROM city ) and ID &lt;&gt; 'matchbook' IN table city</t>
+          <t>FIND store . address_id , manager_staff_id where manager_staff_id = 'Eugene' FROM the store table LIMIT 28 HAVING COUNT ( address_id ) &lt; 95</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT LAST_UPDATE, CITY.POPULATION FROM CITY WHERE COUNTRYCODE IN(SELECT DISTRICT FROM CITY) AND ID &lt; &gt; 'MATCHBOOK' </t>
+          <t xml:space="preserve">SELECT STORE.ADDRESS_ID, MANAGER_STAFF_ID FROM STORE WHERE MANAGER_STAFF_ID = 'EUGENE' HAVING COUNT(ADDRESS_ID) &lt; 95 LIMIT 28 </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -676,12 +752,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WHAT ARE THE ToDate and count ( FromDate ) IN table Titles as Ts where ToDate &gt; '1951-6-1' GROUP BY AUTOMATICALLY</t>
+          <t>WHAT ARE THE last_update and city . Population where CountryCode IN ( SELECT District FROM city ) and ID &lt;&gt; 'matchbook' IN table city</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT TODATE, COUNT(FROMDATE) FROM TITLES AS TS WHERE TODATE &gt; '1951-6-1' GROUP BY TODATE </t>
+          <t xml:space="preserve">SELECT LAST_UPDATE, CITY.POPULATION FROM CITY WHERE COUNTRYCODE IN(SELECT DISTRICT FROM CITY) AND ID &lt; &gt; 'MATCHBOOK' </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -691,12 +772,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>natural join film with language AND THEN WHAT IS original_language_id and the count of ( replacement_cost ) FROM ( WHAT ARE THE city . Name , Population where Name = 'otherworld' or last_update &lt;&gt; '1976-3-23' FROM the city table as cy ) as film AND THEN FROM table language as le SELECT count ( language_id ) , count ( last_update ) where name = 'Aiken' or last_update &lt;&gt; '1956-11-1' AND THEN GROUP BY AUTOMATIC</t>
+          <t>WHAT ARE THE ToDate and count ( FromDate ) IN table Titles as Ts where ToDate &gt; '1951-6-1' GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT FILM.ORIGINAL_LANGUAGE_ID, COUNT(FILM.REPLACEMENT_COST), COUNT(LE.LANGUAGE_ID), COUNT(LE.LAST_UPDATE) FROM(SELECT CITY.NAME, POPULATION FROM CITY AS CY WHERE NAME = 'OTHERWORLD' OR LAST_UPDATE &lt; &gt; '1976-3-23') AS FILM NATURAL JOIN LANGUAGE AS LE WHERE(LE.NAME = 'AIKEN' OR LE.LAST_UPDATE &lt; &gt; '1956-11-1') GROUP BY FILM.ORIGINAL_LANGUAGE_ID </t>
+          <t xml:space="preserve">SELECT TODATE, COUNT(FROMDATE) FROM TITLES AS TS WHERE TODATE &gt; '1951-6-1' GROUP BY TODATE </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -706,12 +792,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>WHAT ARE THE the count ( city ) , the count ( District ) FROM table city as cy where city &lt;&gt; 'trust' and city_id IN ( SELECT city FROM TABLE city ) GROUP AUTOMATIC</t>
+          <t>natural join film with language AND THEN WHAT IS original_language_id and the count of ( replacement_cost ) FROM ( WHAT ARE THE city . Name , Population where Name = 'otherworld' or last_update &lt;&gt; '1976-3-23' FROM the city table as cy ) as film AND THEN FROM table language as le SELECT count ( language_id ) , count ( last_update ) where name = 'Aiken' or last_update &lt;&gt; '1956-11-1' AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(CITY), COUNT(DISTRICT) FROM CITY AS CY WHERE CITY &lt; &gt; 'TRUST' AND CITY_ID IN(SELECT CITY FROM CITY) GROUP BY </t>
+          <t xml:space="preserve">SELECT FILM.ORIGINAL_LANGUAGE_ID, COUNT(FILM.REPLACEMENT_COST), COUNT(LE.LANGUAGE_ID), COUNT(LE.LAST_UPDATE) FROM(SELECT CITY.NAME, POPULATION FROM CITY AS CY WHERE NAME = 'OTHERWORLD' OR LAST_UPDATE &lt; &gt; '1976-3-23') AS FILM NATURAL JOIN LANGUAGE AS LE WHERE(LE.NAME = 'AIKEN' OR LE.LAST_UPDATE &lt; &gt; '1956-11-1') GROUP BY FILM.ORIGINAL_LANGUAGE_ID </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -721,12 +812,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN FROM city as cy RETRIEVE count ( CountryCode ) , the sum of ( Population ) , last_update and count of ( District ) AND THEN DISPLAY Code and the avg of ( GNP ) IN ( WHAT IS max ( Population ) and ID where Population &lt; 727 IN city as cy HAVING MIN ( ID ) &lt;&gt; 18 ) as country where LifeExpectancy = 479 or LifeExpectancy = 173 AND THEN GROUP AUTOMATIC</t>
+          <t>WHAT ARE THE the count ( city ) , the count ( District ) FROM table city as cy where city &lt;&gt; 'trust' and city_id IN ( SELECT city FROM TABLE city ) GROUP AUTOMATIC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(CY.COUNTRYCODE), SUM(CY.POPULATION), CY.LAST_UPDATE, COUNT(CY.DISTRICT), COUNTRY.CODE, AVG(COUNTRY.GNP) FROM CITY AS CY NATURAL JOIN(SELECT MAX(POPULATION), ID FROM CITY AS CY WHERE POPULATION &lt; 727 HAVING MIN(ID) &lt; &gt; 18) AS COUNTRY WHERE(COUNTRY.LIFEEXPECTANCY = 479 OR COUNTRY.LIFEEXPECTANCY = 173) GROUP BY CY.LAST_UPDATE, COUNTRY.CODE </t>
+          <t xml:space="preserve">SELECT COUNT(CITY), COUNT(DISTRICT) FROM CITY AS CY WHERE CITY &lt; &gt; 'TRUST' AND CITY_ID IN(SELECT CITY FROM CITY) GROUP BY </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -736,12 +832,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RETRIEVE count ( store_id ) , the count ( address_id ) and count ( last_update ) FROM the store table GROUP BY AUTOMATIC</t>
+          <t>natural join city with country AND THEN FROM city as cy RETRIEVE count ( CountryCode ) , the sum of ( Population ) , last_update and count of ( District ) AND THEN DISPLAY Code and the avg of ( GNP ) IN ( WHAT IS max ( Population ) and ID where Population &lt; 727 IN city as cy HAVING MIN ( ID ) &lt;&gt; 18 ) as country where LifeExpectancy = 479 or LifeExpectancy = 173 AND THEN GROUP AUTOMATIC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(STORE_ID), COUNT(ADDRESS_ID), COUNT(LAST_UPDATE) FROM STORE GROUP BY </t>
+          <t xml:space="preserve">SELECT COUNT(CY.COUNTRYCODE), SUM(CY.POPULATION), CY.LAST_UPDATE, COUNT(CY.DISTRICT), COUNTRY.CODE, AVG(COUNTRY.GNP) FROM CITY AS CY NATURAL JOIN(SELECT MAX(POPULATION), ID FROM CITY AS CY WHERE POPULATION &lt; 727 HAVING MIN(ID) &lt; &gt; 18) AS COUNTRY WHERE(COUNTRY.LIFEEXPECTANCY = 479 OR COUNTRY.LIFEEXPECTANCY = 173) GROUP BY CY.LAST_UPDATE, COUNTRY.CODE </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -751,12 +852,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>natural join city with countrylanguage AND THEN WHAT ARE THE country_id and city . District FROM city table AND THEN FROM countrylanguage where Language = 'humpback' WHAT IS the count ( Percentage ) , CountryCode AND THEN GROUP BY AUTOMATIC</t>
+          <t>RETRIEVE count ( store_id ) , the count ( address_id ) and count ( last_update ) FROM the store table GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT CITY.COUNTRY_ID, CITY.DISTRICT, COUNT(COUNTRYLANGUAGE.PERCENTAGE), COUNTRYLANGUAGE.COUNTRYCODE FROM CITY NATURAL JOIN COUNTRYLANGUAGE WHERE(COUNTRYLANGUAGE.LANGUAGE = 'HUMPBACK') GROUP BY CITY.COUNTRY_ID, CITY.DISTRICT, COUNTRYLANGUAGE.COUNTRYCODE </t>
+          <t xml:space="preserve">SELECT COUNT(STORE_ID), COUNT(ADDRESS_ID), COUNT(LAST_UPDATE) FROM STORE GROUP BY </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -766,12 +872,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>join course with department on course . deptId equals department . id AND THEN FROM table course WHAT IS min ( units ) and units , course . id and deptId AND THEN IN the department table RETRIEVE departmentName and id</t>
+          <t>natural join city with countrylanguage AND THEN WHAT ARE THE country_id and city . District FROM city table AND THEN FROM countrylanguage where Language = 'humpback' WHAT IS the count ( Percentage ) , CountryCode AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT MIN(COURSE.UNITS), COURSE.UNITS, COURSE.ID, COURSE.DEPTID, DEPARTMENT.DEPARTMENTNAME, DEPARTMENT.ID FROM COURSE JOIN DEPARTMENT ON COURSE.DEPTID </t>
+          <t xml:space="preserve">SELECT CITY.COUNTRY_ID, CITY.DISTRICT, COUNT(COUNTRYLANGUAGE.PERCENTAGE), COUNTRYLANGUAGE.COUNTRYCODE FROM CITY NATURAL JOIN COUNTRYLANGUAGE WHERE(COUNTRYLANGUAGE.LANGUAGE = 'HUMPBACK') GROUP BY CITY.COUNTRY_ID, CITY.DISTRICT, COUNTRYLANGUAGE.COUNTRYCODE </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -781,12 +892,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FROM the Salaries table as Ss SELECT ToDate and FromDate AND THEN GET Employees . FirstName , count of ( Gender ) , EmployeeNumber IN table Employees as Es where BirthDate &gt;= '1984-4-28' AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATICALLY</t>
+          <t>join course with department on course . deptId equals department . id AND THEN FROM table course WHAT IS min ( units ) and units , course . id and deptId AND THEN IN the department table RETRIEVE departmentName and id</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT SS.TODATE, SS.FROMDATE, EMPLOYEES.FIRSTNAME, COUNT(ES.GENDER), ES.EMPLOYEENUMBER FROM SALARIES AS SS NATURAL JOIN EMPLOYEES AS ES WHERE(ES.BIRTHDATE &gt;= '1984-4-28') GROUP BY SS.TODATE, SS.FROMDATE, EMPLOYEES.FIRSTNAME, ES.EMPLOYEENUMBER </t>
+          <t xml:space="preserve">SELECT MIN(COURSE.UNITS), COURSE.UNITS, COURSE.ID, COURSE.DEPTID, DEPARTMENT.DEPARTMENTNAME, DEPARTMENT.ID FROM COURSE JOIN DEPARTMENT ON COURSE.DEPTID </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -796,12 +912,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FROM store table where store_id = 'Calcutta' and store_id IN ( SELECT last_update IN TABLE store ) PRESENT count ( distinct last_update ) , count of ( store_id ) GROUP AUTOMATICALLY</t>
+          <t>FROM the Salaries table as Ss SELECT ToDate and FromDate AND THEN GET Employees . FirstName , count of ( Gender ) , EmployeeNumber IN table Employees as Es where BirthDate &gt;= '1984-4-28' AND THEN natural join Salaries with Employees AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(DISTINCT LAST_UPDATE), COUNT(STORE_ID) FROM STORE WHERE STORE_ID = 'CALCUTTA' AND STORE_ID IN(SELECT LAST_UPDATE FROM STORE) GROUP BY </t>
+          <t xml:space="preserve">SELECT SS.TODATE, SS.FROMDATE, EMPLOYEES.FIRSTNAME, COUNT(ES.GENDER), ES.EMPLOYEENUMBER FROM SALARIES AS SS NATURAL JOIN EMPLOYEES AS ES WHERE(ES.BIRTHDATE &gt;= '1984-4-28') GROUP BY SS.TODATE, SS.FROMDATE, EMPLOYEES.FIRSTNAME, ES.EMPLOYEENUMBER </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -811,12 +932,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>WHAT ARE THE count of ( Population ) and count ( distinct city_id ) IN city as cy AND THEN FROM countrylanguage table WHAT IS THE sum ( Percentage ) and count ( Percentage ) where Language = 'dieldrin' and Language IN ( DISPLAY CountryCode FROM countrylanguage ) AND THEN natural join city with countrylanguage AND THEN GROUP AUTOMATICALLY</t>
+          <t>FROM store table where store_id = 'Calcutta' and store_id IN ( SELECT last_update IN TABLE store ) PRESENT count ( distinct last_update ) , count of ( store_id ) GROUP AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(CY.POPULATION), COUNT(DISTINCT CY.CITY_ID), SUM(COUNTRYLANGUAGE.PERCENTAGE), COUNT(COUNTRYLANGUAGE.PERCENTAGE) FROM CITY AS CY NATURAL JOIN COUNTRYLANGUAGE WHERE(COUNTRYLANGUAGE.LANGUAGE = 'DIELDRIN' AND COUNTRYLANGUAGE.LANGUAGE IN(SELECT COUNTRYCODE FROM COUNTRYLANGUAGE)) GROUP BY </t>
+          <t xml:space="preserve">SELECT COUNT(DISTINCT LAST_UPDATE), COUNT(STORE_ID) FROM STORE WHERE STORE_ID = 'CALCUTTA' AND STORE_ID IN(SELECT LAST_UPDATE FROM STORE) GROUP BY </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -826,12 +952,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FROM table city as cy where country_id &lt;&gt; 'spectroscopy' GET the count ( city ) and count ( Population ) , city and city_id GROUP AUTOMATIC</t>
+          <t>WHAT ARE THE count of ( Population ) and count ( distinct city_id ) IN city as cy AND THEN FROM countrylanguage table WHAT IS THE sum ( Percentage ) and count ( Percentage ) where Language = 'dieldrin' and Language IN ( DISPLAY CountryCode FROM countrylanguage ) AND THEN natural join city with countrylanguage AND THEN GROUP AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(CITY), COUNT(POPULATION), CITY, CITY_ID FROM CITY AS CY WHERE COUNTRY_ID &lt; &gt; 'SPECTROSCOPY' GROUP BY CITY, CITY_ID </t>
+          <t xml:space="preserve">SELECT COUNT(CY.POPULATION), COUNT(DISTINCT CY.CITY_ID), SUM(COUNTRYLANGUAGE.PERCENTAGE), COUNT(COUNTRYLANGUAGE.PERCENTAGE) FROM CITY AS CY NATURAL JOIN COUNTRYLANGUAGE WHERE(COUNTRYLANGUAGE.LANGUAGE = 'DIELDRIN' AND COUNTRYLANGUAGE.LANGUAGE IN(SELECT COUNTRYCODE FROM COUNTRYLANGUAGE)) GROUP BY </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -841,12 +972,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IN table payment as pt GET last_update , customer_id , payment_id , payment . payment_date HAVING SUM ( payment_date ) &gt; 147</t>
+          <t>FROM table city as cy where country_id &lt;&gt; 'spectroscopy' GET the count ( city ) and count ( Population ) , city and city_id GROUP AUTOMATIC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT LAST_UPDATE, CUSTOMER_ID, PAYMENT_ID, PAYMENT.PAYMENT_DATE FROM PAYMENT AS PT HAVING SUM(PAYMENT_DATE) &gt; 147 </t>
+          <t xml:space="preserve">SELECT COUNT(CITY), COUNT(POPULATION), CITY, CITY_ID FROM CITY AS CY WHERE COUNTRY_ID &lt; &gt; 'SPECTROSCOPY' GROUP BY CITY, CITY_ID </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -856,12 +992,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IN table staff WHAT ARE last_update and staff . password and sum ( active ) where first_name &lt;&gt; 'menstruate' GROUP BY AUTOMATIC</t>
+          <t>IN table payment as pt GET last_update , customer_id , payment_id , payment . payment_date HAVING SUM ( payment_date ) &gt; 147</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT LAST_UPDATE, STAFF.PASSWORD, SUM(ACTIVE) FROM STAFF WHERE FIRST_NAME &lt; &gt; 'MENSTRUATE' GROUP BY LAST_UPDATE, STAFF.PASSWORD </t>
+          <t xml:space="preserve">SELECT LAST_UPDATE, CUSTOMER_ID, PAYMENT_ID, PAYMENT.PAYMENT_DATE FROM PAYMENT AS PT HAVING SUM(PAYMENT_DATE) &gt; 147 </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -871,12 +1012,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DISPLAY count of ( rental_date ) and the count ( last_update ) , count ( distinct last_update ) , rental . last_update FROM rental as rl GROUP BY AUTOMATICALLY</t>
+          <t>IN table staff WHAT ARE last_update and staff . password and sum ( active ) where first_name &lt;&gt; 'menstruate' GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(RENTAL_DATE), COUNT(LAST_UPDATE), COUNT(DISTINCT LAST_UPDATE), RENTAL.LAST_UPDATE FROM RENTAL AS RL GROUP BY RENTAL.LAST_UPDATE </t>
+          <t xml:space="preserve">SELECT LAST_UPDATE, STAFF.PASSWORD, SUM(ACTIVE) FROM STAFF WHERE FIRST_NAME &lt; &gt; 'MENSTRUATE' GROUP BY LAST_UPDATE, STAFF.PASSWORD </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -886,12 +1032,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SELECT city . District and the count of ( country_id ) FROM city GROUP BY AUTOMATICALLY</t>
+          <t>DISPLAY count of ( rental_date ) and the count ( last_update ) , count ( distinct last_update ) , rental . last_update FROM rental as rl GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT CITY.DISTRICT, COUNT(COUNTRY_ID) FROM CITY GROUP BY CITY.DISTRICT </t>
+          <t xml:space="preserve">SELECT COUNT(RENTAL_DATE), COUNT(LAST_UPDATE), COUNT(DISTINCT LAST_UPDATE), RENTAL.LAST_UPDATE FROM RENTAL AS RL GROUP BY RENTAL.LAST_UPDATE </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -901,12 +1052,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>IN the Titles table where EmployeeNumber &lt;&gt; 'certify' or FromDate &lt;&gt; '1996-6-22' PRESENT Titles . EmployeeNumber and the count ( Title ) HAVING COUNT ( EmployeeNumber ) &lt; 66 GROUP BY AUTOMATICALLY</t>
+          <t>SELECT city . District and the count of ( country_id ) FROM city GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT TITLES.EMPLOYEENUMBER, COUNT(TITLE) FROM TITLES WHERE EMPLOYEENUMBER &lt; &gt; 'CERTIFY' OR FROMDATE &lt; &gt; '1996-6-22' GROUP BY TITLES.EMPLOYEENUMBER HAVING COUNT(EMPLOYEENUMBER) &lt; 66 </t>
+          <t xml:space="preserve">SELECT CITY.DISTRICT, COUNT(COUNTRY_ID) FROM CITY GROUP BY CITY.DISTRICT </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -916,12 +1072,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RETRIEVE the count ( EmployeeNumber ) , ToDate , DepartmentManager . EmployeeNumber IN the DepartmentManager table as Dr HAVING MIN ( EmployeeNumber ) &lt; 70 GROUP BY AUTOMATICALLY</t>
+          <t>IN the Titles table where EmployeeNumber &lt;&gt; 'certify' or FromDate &lt;&gt; '1996-6-22' PRESENT Titles . EmployeeNumber and the count ( Title ) HAVING COUNT ( EmployeeNumber ) &lt; 66 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(EMPLOYEENUMBER), TODATE, DEPARTMENTMANAGER.EMPLOYEENUMBER FROM DEPARTMENTMANAGER AS DR GROUP BY TODATE, DEPARTMENTMANAGER.EMPLOYEENUMBER HAVING MIN(EMPLOYEENUMBER) &lt; 70 </t>
+          <t xml:space="preserve">SELECT TITLES.EMPLOYEENUMBER, COUNT(TITLE) FROM TITLES WHERE EMPLOYEENUMBER &lt; &gt; 'CERTIFY' OR FROMDATE &lt; &gt; '1996-6-22' GROUP BY TITLES.EMPLOYEENUMBER HAVING COUNT(EMPLOYEENUMBER) &lt; 66 </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -931,12 +1092,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FIND last_update and city . District FROM city AND THEN WHAT ARE max ( IndepYear ) and avg ( GNPOld ) , last_update FROM country table AND THEN natural join city with country AND THEN GROUP BY AUTOMATIC</t>
+          <t>RETRIEVE the count ( EmployeeNumber ) , ToDate , DepartmentManager . EmployeeNumber IN the DepartmentManager table as Dr HAVING MIN ( EmployeeNumber ) &lt; 70 GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT CITY.LAST_UPDATE, CITY.DISTRICT, MAX(COUNTRY.INDEPYEAR), AVG(COUNTRY.GNPOLD), COUNTRY.LAST_UPDATE FROM CITY NATURAL JOIN COUNTRY GROUP BY CITY.LAST_UPDATE, CITY.DISTRICT, COUNTRY.LAST_UPDATE </t>
+          <t xml:space="preserve">SELECT COUNT(EMPLOYEENUMBER), TODATE, DEPARTMENTMANAGER.EMPLOYEENUMBER FROM DEPARTMENTMANAGER AS DR GROUP BY TODATE, DEPARTMENTMANAGER.EMPLOYEENUMBER HAVING MIN(EMPLOYEENUMBER) &lt; 70 </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -946,12 +1112,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PRESENT count ( distinct DepartmentNumber ) and count of ( EmployeeNumber ) , count ( distinct EmployeeNumber ) FROM table DepartmentManager GROUP AUTOMATICALLY</t>
+          <t>FIND last_update and city . District FROM city AND THEN WHAT ARE max ( IndepYear ) and avg ( GNPOld ) , last_update FROM country table AND THEN natural join city with country AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(DISTINCT DEPARTMENTNUMBER), COUNT(EMPLOYEENUMBER), COUNT(DISTINCT EMPLOYEENUMBER) FROM DEPARTMENTMANAGER GROUP BY </t>
+          <t xml:space="preserve">SELECT CITY.LAST_UPDATE, CITY.DISTRICT, MAX(COUNTRY.INDEPYEAR), AVG(COUNTRY.GNPOLD), COUNTRY.LAST_UPDATE FROM CITY NATURAL JOIN COUNTRY GROUP BY CITY.LAST_UPDATE, CITY.DISTRICT, COUNTRY.LAST_UPDATE </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -961,12 +1132,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IN city where ID IN ( FIND city FROM TABLE city ) RETRIEVE max ( Population ) and CountryCode</t>
+          <t>PRESENT count ( distinct DepartmentNumber ) and count of ( EmployeeNumber ) , count ( distinct EmployeeNumber ) FROM table DepartmentManager GROUP AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT MAX(POPULATION), COUNTRYCODE FROM CITY WHERE ID IN(SELECT CITY FROM CITY) </t>
+          <t xml:space="preserve">SELECT COUNT(DISTINCT DEPARTMENTNUMBER), COUNT(EMPLOYEENUMBER), COUNT(DISTINCT EMPLOYEENUMBER) FROM DEPARTMENTMANAGER GROUP BY </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -976,12 +1152,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>WHAT IS the count ( wheelchairSpaces ) , room . wheelchairSpaces , count ( roomNumber ) and room . floor FROM ( RETRIEVE capacity , max ( capacity ) , roomId FROM courseoffering where courseId = 'awoke' or capacity = 542 LIMIT 39 ) as room where roomNumber &lt;&gt; 'needham' or wheelchairSpaces &lt;= 2004 AND THEN WHAT ARE buildingNumber , id , buildingName IN building table AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP BY AUTOMATIC</t>
+          <t>IN city where ID IN ( FIND city FROM TABLE city ) RETRIEVE max ( Population ) and CountryCode</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">WHAT IS THE COUNT WHEELCHAIRSPACES, ROOM.WHEELCHAIRSPACES, COUNT ROOMNUMBER AND ROOM.FLOOR FROM RETRIEVE CAPACITY, MAX CAPACITY, ROOMID FROM COURSEOFFERING WHERE COURSEID = 'AWOKE' OR CAPACITY = 542 LIMIT 39 AS ROOM WHERE ROOMNUMBER &lt; &gt; 'NEEDHAM' OR WHEELCHAIRSPACES &lt;= 2004 AND THEN WHAT ARE BUILDINGNUMBER, ID, BUILDINGNAME IN BUILDING TABLE AND THEN JOIN ROOM WITH BUILDING ON ROOM.BUILDINGID EQUALS BUILDING.ID AND THEN GROUP BY AUTOMATIC </t>
+          <t xml:space="preserve">SELECT MAX(POPULATION), COUNTRYCODE FROM CITY WHERE ID IN(SELECT CITY FROM CITY) </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -991,12 +1172,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>IN the room table SELECT sum ( capacity ) , id AND THEN IN building as bg DISPLAY building . id , the count of ( buildingNumber ) , building . buildingName and the count of ( buildingNumber ) where buildingName = 'raindrop' or buildingName &lt;&gt; 'circadian' AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP AUTOMATIC HAVING AVG ( buildingName ) &gt; 178</t>
+          <t>WHAT IS the count ( wheelchairSpaces ) , room . wheelchairSpaces , count ( roomNumber ) and room . floor FROM ( RETRIEVE capacity , max ( capacity ) , roomId FROM courseoffering where courseId = 'awoke' or capacity = 542 LIMIT 39 ) as room where roomNumber &lt;&gt; 'needham' or wheelchairSpaces &lt;= 2004 AND THEN WHAT ARE buildingNumber , id , buildingName IN building table AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT SUM(ROOM.CAPACITY), ROOM.ID, BUILDING.ID, COUNT(BG.BUILDINGNUMBER), BUILDING.BUILDINGNAME, COUNT(BG.BUILDINGNUMBER), FROM ROOM JOIN BUILDING AS BG ON ROOM.BUILDINGID WHERE(BG.BUILDINGNAME = 'RAINDROP' OR BG.BUILDINGNAME &lt; &gt; 'CIRCADIAN') </t>
+          <t xml:space="preserve">WHAT IS THE COUNT WHEELCHAIRSPACES, ROOM.WHEELCHAIRSPACES, COUNT ROOMNUMBER AND ROOM.FLOOR FROM RETRIEVE CAPACITY, MAX CAPACITY, ROOMID FROM COURSEOFFERING WHERE COURSEID = 'AWOKE' OR CAPACITY = 542 LIMIT 39 AS ROOM WHERE ROOMNUMBER &lt; &gt; 'NEEDHAM' OR WHEELCHAIRSPACES &lt;= 2004 AND THEN WHAT ARE BUILDINGNUMBER, ID, BUILDINGNAME IN BUILDING TABLE AND THEN JOIN ROOM WITH BUILDING ON ROOM.BUILDINGID EQUALS BUILDING.ID AND THEN GROUP BY AUTOMATIC </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>PARTIAL ERROR</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1192,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>WHAT ARE THE last_update and inventory . film_id , count ( inventory_id ) , inventory . inventory_id FROM the inventory table as iy GROUP AUTOMATIC HAVING MAX ( last_update ) &lt;&gt; 187</t>
+          <t>IN the room table SELECT sum ( capacity ) , id AND THEN IN building as bg DISPLAY building . id , the count of ( buildingNumber ) , building . buildingName and the count of ( buildingNumber ) where buildingName = 'raindrop' or buildingName &lt;&gt; 'circadian' AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP AUTOMATIC HAVING AVG ( buildingName ) &gt; 178</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT LAST_UPDATE, INVENTORY.FILM_ID, COUNT(INVENTORY_ID), INVENTORY.INVENTORY_ID FROM INVENTORY AS IY GROUP BY LAST_UPDATE, INVENTORY.FILM_ID, INVENTORY.INVENTORY_ID HAVING MAX(LAST_UPDATE) &lt; &gt; 187 </t>
+          <t xml:space="preserve">SELECT SUM(ROOM.CAPACITY), ROOM.ID, BUILDING.ID, COUNT(BG.BUILDINGNUMBER), BUILDING.BUILDINGNAME, COUNT(BG.BUILDINGNUMBER), FROM ROOM JOIN BUILDING AS BG ON ROOM.BUILDINGID WHERE(BG.BUILDINGNAME = 'RAINDROP' OR BG.BUILDINGNAME &lt; &gt; 'CIRCADIAN') </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1212,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FROM table room GET the count ( wheelchairSpaces ) , capacity where wheelchairSpaces = 842 or id = 'thoriate' AND THEN FROM ( IN table term as tm FIND avg ( year ) , the count of ( id ) and year , endDate GROUP BY AUTOMATIC HAVING SUM ( endDate ) &lt; 134 ) as building where id = 'Cromwellian' SELECT building . buildingNumber and building . id and buildingName AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP BY AUTOMATICALLY</t>
+          <t>WHAT ARE THE last_update and inventory . film_id , count ( inventory_id ) , inventory . inventory_id FROM the inventory table as iy GROUP AUTOMATIC HAVING MAX ( last_update ) &lt;&gt; 187</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(ROOM.WHEELCHAIRSPACES), ROOM.CAPACITY FROM ROOM JOIN BUILDING ON ROOM.BUILDINGID WHERE(ROOM.WHEELCHAIRSPACES = 842 OR ROOM.ID = 'THORIATE') </t>
+          <t xml:space="preserve">SELECT LAST_UPDATE, INVENTORY.FILM_ID, COUNT(INVENTORY_ID), INVENTORY.INVENTORY_ID FROM INVENTORY AS IY GROUP BY LAST_UPDATE, INVENTORY.FILM_ID, INVENTORY.INVENTORY_ID HAVING MAX(LAST_UPDATE) &lt; &gt; 187 </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1232,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PRESENT CountryCode and Name where country_id IN ( DISPLAY country_id FROM TABLE city ) FROM the city table HAVING AVG ( Name ) &lt; 159</t>
+          <t>FROM table room GET the count ( wheelchairSpaces ) , capacity where wheelchairSpaces = 842 or id = 'thoriate' AND THEN FROM ( IN table term as tm FIND avg ( year ) , the count of ( id ) and year , endDate GROUP BY AUTOMATIC HAVING SUM ( endDate ) &lt; 134 ) as building where id = 'Cromwellian' SELECT building . buildingNumber and building . id and buildingName AND THEN join room with building on room . buildingId equals building . id AND THEN GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNTRYCODE, NAME FROM CITY WHERE COUNTRY_ID IN(SELECT COUNTRY_ID FROM CITY) HAVING AVG(NAME) &lt; 159 </t>
+          <t xml:space="preserve">SELECT COUNT(ROOM.WHEELCHAIRSPACES), ROOM.CAPACITY FROM ROOM JOIN BUILDING ON ROOM.BUILDINGID WHERE(ROOM.WHEELCHAIRSPACES = 842 OR ROOM.ID = 'THORIATE') </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1051,12 +1252,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>natural join city with country AND THEN WHAT ARE THE city . city and last_update FROM city as cy AND THEN PRESENT country and avg ( Population ) FROM table country AND THEN HAVING MIN ( country ) &gt; 101 GROUP BY AUTOMATIC</t>
+          <t>PRESENT CountryCode and Name where country_id IN ( DISPLAY country_id FROM TABLE city ) FROM the city table HAVING AVG ( Name ) &lt; 159</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT CITY.CITY, CY.LAST_UPDATE, COUNTRY.COUNTRY, AVG(COUNTRY.POPULATION) FROM CITY AS CY NATURAL JOIN COUNTRY GROUP BY CITY.CITY, CY.LAST_UPDATE, COUNTRY.COUNTRY HAVING MIN(COUNTRY) &gt; 101 </t>
+          <t xml:space="preserve">SELECT COUNTRYCODE, NAME FROM CITY WHERE COUNTRY_ID IN(SELECT COUNTRY_ID FROM CITY) HAVING AVG(NAME) &lt; 159 </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1272,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FROM table courseoffering as cg PRESENT sum ( capacity ) and courseoffering . id GROUP BY AUTOMATICALLY</t>
+          <t>natural join city with country AND THEN WHAT ARE THE city . city and last_update FROM city as cy AND THEN PRESENT country and avg ( Population ) FROM table country AND THEN HAVING MIN ( country ) &gt; 101 GROUP BY AUTOMATIC</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT SUM(CAPACITY), COURSEOFFERING.ID FROM COURSEOFFERING AS CG GROUP BY COURSEOFFERING.ID </t>
+          <t xml:space="preserve">SELECT CITY.CITY, CY.LAST_UPDATE, COUNTRY.COUNTRY, AVG(COUNTRY.POPULATION) FROM CITY AS CY NATURAL JOIN COUNTRY GROUP BY CITY.CITY, CY.LAST_UPDATE, COUNTRY.COUNTRY HAVING MIN(COUNTRY) &gt; 101 </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1292,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>natural join DepartmentManager with departments AND THEN FROM the DepartmentManager table as Dr DISPLAY the count ( ToDate ) and EmployeeNumber , count ( FromDate ) AND THEN IN departments as ds where DepartmentName = 'churchmen' and DepartmentNumber &lt;&gt; 'quonset' SHOW ME DepartmentNumber , DepartmentName AND THEN GROUP AUTOMATICALLY LIMIT 3</t>
+          <t>FROM table courseoffering as cg PRESENT sum ( capacity ) and courseoffering . id GROUP BY AUTOMATICALLY</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(DR.TODATE), DR.EMPLOYEENUMBER, COUNT(DR.FROMDATE), DS.DEPARTMENTNUMBER, DS.DEPARTMENTNAME FROM DEPARTMENTMANAGER AS DR NATURAL JOIN DEPARTMENTS AS DS WHERE(DS.DEPARTMENTNAME = 'CHURCHMEN' AND DS.DEPARTMENTNUMBER &lt; &gt; 'QUONSET') GROUP BY DR.EMPLOYEENUMBER, DS.DEPARTMENTNUMBER, DS.DEPARTMENTNAME LIMIT 3 </t>
+          <t xml:space="preserve">SELECT SUM(CAPACITY), COURSEOFFERING.ID FROM COURSEOFFERING AS CG GROUP BY COURSEOFFERING.ID </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1096,12 +1312,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FROM film table WHAT IS THE film . rating and rental_rate , count ( last_update ) GROUP AUTOMATICALLY HAVING MIN ( rental_rate ) = 44</t>
+          <t>natural join DepartmentManager with departments AND THEN FROM the DepartmentManager table as Dr DISPLAY the count ( ToDate ) and EmployeeNumber , count ( FromDate ) AND THEN IN departments as ds where DepartmentName = 'churchmen' and DepartmentNumber &lt;&gt; 'quonset' SHOW ME DepartmentNumber , DepartmentName AND THEN GROUP AUTOMATICALLY LIMIT 3</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT FILM.RATING, RENTAL_RATE, COUNT(LAST_UPDATE) FROM FILM GROUP BY FILM.RATING, RENTAL_RATE HAVING MIN(RENTAL_RATE) = 44 </t>
+          <t xml:space="preserve">SELECT COUNT(DR.TODATE), DR.EMPLOYEENUMBER, COUNT(DR.FROMDATE), DS.DEPARTMENTNUMBER, DS.DEPARTMENTNAME FROM DEPARTMENTMANAGER AS DR NATURAL JOIN DEPARTMENTS AS DS WHERE(DS.DEPARTMENTNAME = 'CHURCHMEN' AND DS.DEPARTMENTNUMBER &lt; &gt; 'QUONSET') GROUP BY DR.EMPLOYEENUMBER, DS.DEPARTMENTNUMBER, DS.DEPARTMENTNAME LIMIT 3 </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1332,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>IN the city table DISPLAY city . ID and city . Name , city . city HAVING MAX ( city ) &gt; 80</t>
+          <t>FROM film table WHAT IS THE film . rating and rental_rate , count ( last_update ) GROUP AUTOMATICALLY HAVING MIN ( rental_rate ) = 44</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT CITY.ID, CITY.NAME, CITY.CITY FROM CITY HAVING MAX(CITY) &gt; 80 </t>
+          <t xml:space="preserve">SELECT FILM.RATING, RENTAL_RATE, COUNT(LAST_UPDATE) FROM FILM GROUP BY FILM.RATING, RENTAL_RATE HAVING MIN(RENTAL_RATE) = 44 </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1126,10 +1352,19 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FROM the term table DISPLAY term . startDate and endDate AND THEN natural join term with term</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
+          <t>IN the city table DISPLAY city . ID and city . Name , city . city HAVING MAX ( city ) &gt; 80</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SELECT CITY.ID, CITY.NAME, CITY.CITY FROM CITY HAVING MAX(CITY) &gt; 80 </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1137,12 +1372,13 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>natural join DepartmentEmployee with departments AND THEN IN table DepartmentEmployee where FromDate &gt; '1998-9-21' SELECT ToDate and DepartmentNumber AND THEN IN the departments table FIND departments . DepartmentName , DepartmentNumber where DepartmentNumber &lt;&gt; 'desperate' or DepartmentName &lt;&gt; 'bled'</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SELECT DEPARTMENTEMPLOYEE.TODATE, DEPARTMENTEMPLOYEE.DEPARTMENTNUMBER, DEPARTMENTS.DEPARTMENTNAME, DEPARTMENTS.DEPARTMENTNUMBER FROM DEPARTMENTEMPLOYEE NATURAL JOIN DEPARTMENTS WHERE(DEPARTMENTEMPLOYEE.FROMDATE &gt; '1998-9-21') AND(DEPARTMENTS.DEPARTMENTNUMBER &lt; &gt; 'DESPERATE' OR DEPARTMENTS.DEPARTMENTNAME &lt; &gt; 'BLED') </t>
+          <t>FROM the term table DISPLAY term . startDate and endDate AND THEN natural join term with term</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>PARTIAL ERROR</t>
         </is>
       </c>
     </row>
@@ -1152,12 +1388,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FROM table term WHAT ARE THE the count ( startDate ) and count ( termPeriod ) , term . startDate GROUP BY AUTOMATIC</t>
+          <t>natural join DepartmentEmployee with departments AND THEN IN table DepartmentEmployee where FromDate &gt; '1998-9-21' SELECT ToDate and DepartmentNumber AND THEN IN the departments table FIND departments . DepartmentName , DepartmentNumber where DepartmentNumber &lt;&gt; 'desperate' or DepartmentName &lt;&gt; 'bled'</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">SELECT COUNT(STARTDATE), COUNT(TERMPERIOD), TERM.STARTDATE FROM TERM GROUP BY TERM.STARTDATE </t>
+          <t xml:space="preserve">SELECT DEPARTMENTEMPLOYEE.TODATE, DEPARTMENTEMPLOYEE.DEPARTMENTNUMBER, DEPARTMENTS.DEPARTMENTNAME, DEPARTMENTS.DEPARTMENTNUMBER FROM DEPARTMENTEMPLOYEE NATURAL JOIN DEPARTMENTS WHERE(DEPARTMENTEMPLOYEE.FROMDATE &gt; '1998-9-21') AND(DEPARTMENTS.DEPARTMENTNUMBER &lt; &gt; 'DESPERATE' OR DEPARTMENTS.DEPARTMENTNAME &lt; &gt; 'BLED') </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>
@@ -1167,12 +1408,37 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>FROM table term WHAT ARE THE the count ( startDate ) and count ( termPeriod ) , term . startDate GROUP BY AUTOMATIC</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SELECT COUNT(STARTDATE), COUNT(TERMPERIOD), TERM.STARTDATE FROM TERM GROUP BY TERM.STARTDATE </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>join store with staff on store . manager_staff_id equals staff . staff_id AND THEN WHAT ARE count of ( manager_staff_id ) and address_id IN table store as se where store_id = 'abstract' and address_id IN ( FIND manager_staff_id FROM staff ) AND THEN GET last_update , active and staff . address_id where active &gt;= 482 or staff_id &lt;&gt; 'cherubim' IN the staff table AND THEN GROUP BY AUTOMATIC HAVING SUM ( last_update ) &lt; 104 LIMIT 13</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">SELECT COUNT(SE.MANAGER_STAFF_ID), SE.ADDRESS_ID, STAFF.LAST_UPDATE, STAFF.ACTIVE, STAFF.ADDRESS_ID FROM STORE AS SE JOIN STAFF ON STORE.MANAGER_STAFF_ID WHERE(SE.STORE_ID = 'ABSTRACT' AND SE.ADDRESS_ID IN(SELECT MANAGER_STAFF_ID FROM STAFF)) AND(STAFF.ACTIVE &gt;= 482 OR STAFF.STAFF_ID &lt; &gt; 'CHERUBIM') GROUP BY SE.ADDRESS_ID, STAFF.LAST_UPDATE, STAFF.ACTIVE, STAFF.ADDRESS_ID HAVING SUM(LAST_UPDATE) &lt; 104 LIMIT 13 </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>TRANSLATED</t>
         </is>
       </c>
     </row>

</xml_diff>